<commit_message>
Update login and logout functionalities; set headless mode for tests
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF302B0-FD27-49B4-9E7C-0EC1BD0D57C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3FB51F-FCF3-4F31-BEFA-402B4498B2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Enhance test framework: refactor configuration, improve page object methods, and update login/logout processes
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3FB51F-FCF3-4F31-BEFA-402B4498B2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF60315A-C1DD-4903-9976-989E3328AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -39,9 +39,6 @@
     <t>TC0001</t>
   </si>
   <si>
-    <t>My Account</t>
-  </si>
-  <si>
     <t>TestCaseName</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>Pantene Pro-V</t>
-  </si>
-  <si>
-    <t>PageTitleMyAccountPage</t>
   </si>
   <si>
     <t>TC0002</t>
@@ -221,11 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D74549-BFE5-4812-9BD3-EF4C8BA9C7C8}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,13 +510,12 @@
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -531,10 +523,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -542,11 +534,8 @@
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -554,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -565,146 +554,125 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functionality to manage shopping cart: implement product deletion and enhance test cases for adding and verifying products
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF60315A-C1DD-4903-9976-989E3328AC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DE5D1-B429-4E98-9059-61E0FF96DA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="2" r:id="rId1"/>
+    <sheet name="DeleteProduct" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -151,6 +152,12 @@
   </si>
   <si>
     <t>Secret Obsession Perfume</t>
+  </si>
+  <si>
+    <t>Delete Pantene Pro-V Product from Shopping Cart</t>
+  </si>
+  <si>
+    <t>Delete Shaving cream Product from Shopping Cart</t>
   </si>
 </sst>
 </file>
@@ -501,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D74549-BFE5-4812-9BD3-EF4C8BA9C7C8}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,4 +686,67 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB8FB28-8B62-4B49-8E33-4E825B11191B}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement checkout functionality: add CheckoutConfirmationPage, enhance shopping cart tests, and refactor UI actions for better reporting
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063DE5D1-B429-4E98-9059-61E0FF96DA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF28D379-2A63-4125-8CFD-2819852CF28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>New French With Ease</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>Add Makeup Product to Shopping Cart</t>
@@ -508,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D74549-BFE5-4812-9BD3-EF4C8BA9C7C8}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -584,27 +587,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -616,15 +619,15 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -636,21 +639,21 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>24</v>
@@ -664,22 +667,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB8FB28-8B62-4B49-8E33-4E825B11191B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -726,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -740,10 +743,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test configurations and add product management tests: enable headless mode, add tests for adding and deleting products from the shopping cart, and update state.json for consistent test execution.
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF28D379-2A63-4125-8CFD-2819852CF28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71ED6E7-47EC-40DB-A70C-FE4966AE2992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>New French With Ease</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Add Makeup Product to Shopping Cart</t>
@@ -512,7 +509,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +564,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -587,27 +584,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -619,15 +616,15 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -639,21 +636,21 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>24</v>
@@ -667,22 +664,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -743,10 +740,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add wishlist functionality: implement MyWishlistPage, enhance ProductDetailsPage for wishlist actions, and update tests for adding and deleting products from wishlist
</commit_message>
<xml_diff>
--- a/test-data/test-data-automation-test-store.xlsx
+++ b/test-data/test-data-automation-test-store.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PlaywrightE2EAutomation\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71ED6E7-47EC-40DB-A70C-FE4966AE2992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BB93B5-401E-47AF-9EDA-8B9E7FB07767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddProduct" sheetId="2" r:id="rId1"/>
-    <sheet name="DeleteProduct" sheetId="3" r:id="rId2"/>
+    <sheet name="AddProductShoppingCart" sheetId="2" r:id="rId1"/>
+    <sheet name="AddProductWishlist" sheetId="4" r:id="rId2"/>
+    <sheet name="DeleteProductFromShoppingCart" sheetId="3" r:id="rId3"/>
+    <sheet name="DeleteProductFromWishlist" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
   <si>
     <t>ExecutionFlag</t>
   </si>
@@ -158,6 +160,33 @@
   </si>
   <si>
     <t>Delete Shaving cream Product from Shopping Cart</t>
+  </si>
+  <si>
+    <t>Add Hair Care Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Apparel &amp; accessories Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Makeup Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Skincare Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Mens Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Books Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Add Fragrance Product to Wishlist</t>
+  </si>
+  <si>
+    <t>Delete Pantene Pro-V Product from Wish list</t>
+  </si>
+  <si>
+    <t>Delete Shaving cream Product from Wish list</t>
   </si>
 </sst>
 </file>
@@ -508,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D74549-BFE5-4812-9BD3-EF4C8BA9C7C8}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,11 +718,194 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16507A2F-41B2-48A7-B4E0-8DCEFE318C0A}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB8FB28-8B62-4B49-8E33-4E825B11191B}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,4 +961,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDFD2F4-5529-4189-9495-8121C614EB51}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>